<commit_message>
README update + events update until 29/02/2020
</commit_message>
<xml_diff>
--- a/covid19_events.xlsx
+++ b/covid19_events.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cganty\Documents\src\GitHub\COVID-19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05FB315-2C75-4448-B45B-5AB8C5A684EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0E07E9-EFD1-4DC6-B1C4-CEFCC4737666}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10335" windowHeight="10920" xr2:uid="{21C70E2E-B89D-4ECD-8147-7A21A676BFAC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{21C70E2E-B89D-4ECD-8147-7A21A676BFAC}"/>
   </bookViews>
   <sheets>
     <sheet name="events" sheetId="1" r:id="rId1"/>
     <sheet name="label" sheetId="2" r:id="rId2"/>
     <sheet name="iso2" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="source" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">events!$C$1:$C$122</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">events!$C$1:$C$123</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1067" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1170" uniqueCount="383">
   <si>
     <t>id</t>
   </si>
@@ -1129,6 +1129,63 @@
   </si>
   <si>
     <t>c82000o</t>
+  </si>
+  <si>
+    <t>over 2800 deaths</t>
+  </si>
+  <si>
+    <t>d2800o</t>
+  </si>
+  <si>
+    <t>650 positive-cases</t>
+  </si>
+  <si>
+    <t>c650</t>
+  </si>
+  <si>
+    <t>expand President rights for industrial production rise</t>
+  </si>
+  <si>
+    <t>2 positive-cases</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>3150 positive-cases</t>
+  </si>
+  <si>
+    <t>c3150</t>
+  </si>
+  <si>
+    <t>593 positive-cases</t>
+  </si>
+  <si>
+    <t>c593</t>
+  </si>
+  <si>
+    <t>43 deaths</t>
+  </si>
+  <si>
+    <t>d43</t>
+  </si>
+  <si>
+    <t>388 positive-cases</t>
+  </si>
+  <si>
+    <t>c388</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>3 positive-cases</t>
+  </si>
+  <si>
+    <t>c3</t>
   </si>
 </sst>
 </file>
@@ -1152,18 +1209,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1183,9 +1234,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1501,10 +1552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE82E1A5-1AF0-4B8D-AEC0-EAE4D7F581D4}">
-  <dimension ref="A1:M161"/>
+  <dimension ref="A1:M186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G146" workbookViewId="0">
-      <selection activeCell="H157" sqref="H157"/>
+    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
+      <selection activeCell="C177" sqref="C177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1576,10 +1627,10 @@
         <v>43830</v>
       </c>
       <c r="F2" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" t="s">
         <v>70</v>
-      </c>
-      <c r="G2" t="s">
-        <v>173</v>
       </c>
       <c r="H2" t="s">
         <v>73</v>
@@ -2232,7 +2283,9 @@
       <c r="L23" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="M23" s="1"/>
+      <c r="M23" s="1">
+        <v>43911</v>
+      </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -2686,10 +2739,10 @@
       <c r="H38" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="L38" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M38" s="1">
+      <c r="L38" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="M38" s="4">
         <v>43911</v>
       </c>
     </row>
@@ -5317,67 +5370,64 @@
         <v>43911</v>
       </c>
     </row>
-    <row r="122" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="3">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A122">
         <v>121</v>
       </c>
-      <c r="B122" s="3">
+      <c r="B122">
         <v>121</v>
       </c>
-      <c r="C122" s="3" t="s">
+      <c r="C122" t="s">
         <v>12</v>
       </c>
-      <c r="D122" s="4">
-        <v>43882</v>
-      </c>
-      <c r="F122" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G122" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H122" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="I122" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="L122" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="M122" s="4">
-        <v>43911</v>
-      </c>
-    </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F122" t="s">
+        <v>81</v>
+      </c>
+      <c r="G122" t="s">
+        <v>84</v>
+      </c>
+      <c r="H122" t="s">
+        <v>381</v>
+      </c>
+      <c r="I122" t="s">
+        <v>382</v>
+      </c>
+      <c r="L122" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M122" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
       <c r="B123">
         <v>122</v>
       </c>
-      <c r="C123" t="s">
-        <v>39</v>
-      </c>
-      <c r="D123" s="1">
-        <v>43883</v>
-      </c>
-      <c r="F123" t="s">
-        <v>81</v>
-      </c>
-      <c r="G123" t="s">
-        <v>84</v>
-      </c>
-      <c r="H123" t="s">
-        <v>236</v>
-      </c>
-      <c r="I123" t="s">
-        <v>346</v>
-      </c>
-      <c r="L123" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M123" s="1">
+      <c r="C123" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D123" s="4">
+        <v>43882</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G123" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H123" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="I123" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="L123" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="M123" s="4">
         <v>43911</v>
       </c>
     </row>
@@ -5389,7 +5439,7 @@
         <v>123</v>
       </c>
       <c r="C124" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="D124" s="1">
         <v>43883</v>
@@ -5398,13 +5448,13 @@
         <v>81</v>
       </c>
       <c r="G124" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H124" t="s">
-        <v>225</v>
+        <v>236</v>
       </c>
       <c r="I124" t="s">
-        <v>280</v>
+        <v>346</v>
       </c>
       <c r="L124" s="2" t="s">
         <v>71</v>
@@ -5421,7 +5471,7 @@
         <v>124</v>
       </c>
       <c r="C125" t="s">
-        <v>223</v>
+        <v>12</v>
       </c>
       <c r="D125" s="1">
         <v>43883</v>
@@ -5430,13 +5480,13 @@
         <v>81</v>
       </c>
       <c r="G125" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H125" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="I125" t="s">
-        <v>347</v>
+        <v>280</v>
       </c>
       <c r="L125" s="2" t="s">
         <v>71</v>
@@ -5462,13 +5512,13 @@
         <v>81</v>
       </c>
       <c r="G126" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H126" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I126" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="L126" s="2" t="s">
         <v>71</v>
@@ -5497,10 +5547,10 @@
         <v>79</v>
       </c>
       <c r="H127" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="I127" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="L127" s="2" t="s">
         <v>71</v>
@@ -5517,7 +5567,7 @@
         <v>127</v>
       </c>
       <c r="C128" t="s">
-        <v>68</v>
+        <v>223</v>
       </c>
       <c r="D128" s="1">
         <v>43883</v>
@@ -5526,13 +5576,13 @@
         <v>81</v>
       </c>
       <c r="G128" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H128" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I128" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L128" s="2" t="s">
         <v>71</v>
@@ -5548,17 +5598,23 @@
       <c r="B129">
         <v>128</v>
       </c>
+      <c r="C129" t="s">
+        <v>68</v>
+      </c>
       <c r="D129" s="1">
-        <v>43884</v>
+        <v>43883</v>
       </c>
       <c r="F129" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="G129" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="H129" t="s">
-        <v>241</v>
+        <v>240</v>
+      </c>
+      <c r="I129" t="s">
+        <v>350</v>
       </c>
       <c r="L129" s="2" t="s">
         <v>71</v>
@@ -5574,23 +5630,17 @@
       <c r="B130">
         <v>129</v>
       </c>
-      <c r="C130" t="s">
-        <v>12</v>
-      </c>
       <c r="D130" s="1">
         <v>43884</v>
       </c>
       <c r="F130" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="G130" t="s">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="H130" t="s">
-        <v>242</v>
-      </c>
-      <c r="I130" t="s">
-        <v>281</v>
+        <v>241</v>
       </c>
       <c r="L130" s="2" t="s">
         <v>71</v>
@@ -5613,13 +5663,16 @@
         <v>43884</v>
       </c>
       <c r="F131" t="s">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="G131" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="H131" t="s">
-        <v>243</v>
+        <v>242</v>
+      </c>
+      <c r="I131" t="s">
+        <v>281</v>
       </c>
       <c r="L131" s="2" t="s">
         <v>71</v>
@@ -5636,22 +5689,19 @@
         <v>131</v>
       </c>
       <c r="C132" t="s">
-        <v>244</v>
+        <v>12</v>
       </c>
       <c r="D132" s="1">
-        <v>43885</v>
+        <v>43884</v>
       </c>
       <c r="F132" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="G132" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="H132" t="s">
-        <v>132</v>
-      </c>
-      <c r="I132" t="s">
-        <v>99</v>
+        <v>243</v>
       </c>
       <c r="L132" s="2" t="s">
         <v>71</v>
@@ -5668,7 +5718,7 @@
         <v>132</v>
       </c>
       <c r="C133" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D133" s="1">
         <v>43885</v>
@@ -5700,7 +5750,7 @@
         <v>133</v>
       </c>
       <c r="C134" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D134" s="1">
         <v>43885</v>
@@ -5732,7 +5782,7 @@
         <v>134</v>
       </c>
       <c r="C135" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D135" s="1">
         <v>43885</v>
@@ -5764,7 +5814,7 @@
         <v>135</v>
       </c>
       <c r="C136" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D136" s="1">
         <v>43885</v>
@@ -5796,7 +5846,7 @@
         <v>136</v>
       </c>
       <c r="C137" t="s">
-        <v>39</v>
+        <v>252</v>
       </c>
       <c r="D137" s="1">
         <v>43885</v>
@@ -5808,10 +5858,10 @@
         <v>84</v>
       </c>
       <c r="H137" t="s">
-        <v>255</v>
+        <v>132</v>
       </c>
       <c r="I137" t="s">
-        <v>351</v>
+        <v>99</v>
       </c>
       <c r="L137" s="2" t="s">
         <v>71</v>
@@ -5837,13 +5887,13 @@
         <v>81</v>
       </c>
       <c r="G138" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H138" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I138" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L138" s="2" t="s">
         <v>71</v>
@@ -5860,7 +5910,7 @@
         <v>138</v>
       </c>
       <c r="C139" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="D139" s="1">
         <v>43885</v>
@@ -5872,10 +5922,10 @@
         <v>79</v>
       </c>
       <c r="H139" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I139" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L139" s="2" t="s">
         <v>71</v>
@@ -5901,13 +5951,13 @@
         <v>81</v>
       </c>
       <c r="G140" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H140" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I140" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="L140" s="2" t="s">
         <v>71</v>
@@ -5924,7 +5974,7 @@
         <v>140</v>
       </c>
       <c r="C141" t="s">
-        <v>12</v>
+        <v>68</v>
       </c>
       <c r="D141" s="1">
         <v>43885</v>
@@ -5933,13 +5983,13 @@
         <v>81</v>
       </c>
       <c r="G141" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H141" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="I141" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="L141" s="2" t="s">
         <v>71</v>
@@ -5956,22 +6006,22 @@
         <v>141</v>
       </c>
       <c r="C142" t="s">
-        <v>223</v>
+        <v>12</v>
       </c>
       <c r="D142" s="1">
-        <v>43886</v>
+        <v>43885</v>
       </c>
       <c r="F142" t="s">
         <v>81</v>
       </c>
       <c r="G142" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H142" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="I142" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="L142" s="2" t="s">
         <v>71</v>
@@ -5997,13 +6047,13 @@
         <v>81</v>
       </c>
       <c r="G143" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H143" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I143" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="L143" s="2" t="s">
         <v>71</v>
@@ -6014,13 +6064,13 @@
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="B144">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C144" t="s">
-        <v>68</v>
+        <v>223</v>
       </c>
       <c r="D144" s="1">
         <v>43886</v>
@@ -6032,10 +6082,10 @@
         <v>79</v>
       </c>
       <c r="H144" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I144" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="L144" s="2" t="s">
         <v>71</v>
@@ -6046,10 +6096,10 @@
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="B145">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C145" t="s">
         <v>68</v>
@@ -6061,13 +6111,13 @@
         <v>81</v>
       </c>
       <c r="G145" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H145" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I145" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="L145" s="2" t="s">
         <v>71</v>
@@ -6084,7 +6134,7 @@
         <v>145</v>
       </c>
       <c r="C146" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="D146" s="1">
         <v>43886</v>
@@ -6096,10 +6146,10 @@
         <v>84</v>
       </c>
       <c r="H146" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I146" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="L146" s="2" t="s">
         <v>71</v>
@@ -6116,7 +6166,7 @@
         <v>146</v>
       </c>
       <c r="C147" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="D147" s="1">
         <v>43886</v>
@@ -6128,10 +6178,10 @@
         <v>84</v>
       </c>
       <c r="H147" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I147" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="L147" s="2" t="s">
         <v>71</v>
@@ -6148,22 +6198,22 @@
         <v>147</v>
       </c>
       <c r="C148" t="s">
-        <v>106</v>
+        <v>12</v>
       </c>
       <c r="D148" s="1">
-        <v>43887</v>
+        <v>43886</v>
       </c>
       <c r="F148" t="s">
         <v>81</v>
       </c>
       <c r="G148" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="H148" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I148" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L148" s="2" t="s">
         <v>71</v>
@@ -6189,13 +6239,13 @@
         <v>81</v>
       </c>
       <c r="G149" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="H149" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I149" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L149" s="2" t="s">
         <v>71</v>
@@ -6212,7 +6262,7 @@
         <v>149</v>
       </c>
       <c r="C150" t="s">
-        <v>267</v>
+        <v>106</v>
       </c>
       <c r="D150" s="1">
         <v>43887</v>
@@ -6224,10 +6274,10 @@
         <v>84</v>
       </c>
       <c r="H150" t="s">
-        <v>132</v>
+        <v>266</v>
       </c>
       <c r="I150" t="s">
-        <v>99</v>
+        <v>362</v>
       </c>
       <c r="L150" s="2" t="s">
         <v>71</v>
@@ -6244,7 +6294,7 @@
         <v>150</v>
       </c>
       <c r="C151" t="s">
-        <v>29</v>
+        <v>267</v>
       </c>
       <c r="D151" s="1">
         <v>43887</v>
@@ -6276,7 +6326,7 @@
         <v>151</v>
       </c>
       <c r="C152" t="s">
-        <v>269</v>
+        <v>29</v>
       </c>
       <c r="D152" s="1">
         <v>43887</v>
@@ -6308,7 +6358,7 @@
         <v>152</v>
       </c>
       <c r="C153" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D153" s="1">
         <v>43887</v>
@@ -6340,7 +6390,7 @@
         <v>153</v>
       </c>
       <c r="C154" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D154" s="1">
         <v>43887</v>
@@ -6372,7 +6422,7 @@
         <v>154</v>
       </c>
       <c r="C155" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D155" s="1">
         <v>43887</v>
@@ -6404,7 +6454,7 @@
         <v>155</v>
       </c>
       <c r="C156" t="s">
-        <v>254</v>
+        <v>275</v>
       </c>
       <c r="D156" s="1">
         <v>43887</v>
@@ -6436,10 +6486,10 @@
         <v>156</v>
       </c>
       <c r="C157" t="s">
-        <v>32</v>
+        <v>254</v>
       </c>
       <c r="D157" s="1">
-        <v>43888</v>
+        <v>43887</v>
       </c>
       <c r="F157" t="s">
         <v>81</v>
@@ -6468,7 +6518,7 @@
         <v>157</v>
       </c>
       <c r="C158" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="D158" s="1">
         <v>43888</v>
@@ -6500,7 +6550,7 @@
         <v>158</v>
       </c>
       <c r="C159" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D159" s="1">
         <v>43888</v>
@@ -6516,6 +6566,12 @@
       </c>
       <c r="I159" t="s">
         <v>99</v>
+      </c>
+      <c r="L159" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M159" s="1">
+        <v>43911</v>
       </c>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.25">
@@ -6526,7 +6582,7 @@
         <v>159</v>
       </c>
       <c r="C160" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D160" s="1">
         <v>43888</v>
@@ -6543,26 +6599,661 @@
       <c r="I160" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="161" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="L160" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M160" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A161">
+        <v>160</v>
+      </c>
+      <c r="B161">
+        <v>160</v>
+      </c>
       <c r="C161" t="s">
+        <v>17</v>
+      </c>
+      <c r="D161" s="1">
+        <v>43888</v>
+      </c>
+      <c r="F161" t="s">
+        <v>81</v>
+      </c>
+      <c r="G161" t="s">
+        <v>84</v>
+      </c>
+      <c r="H161" t="s">
+        <v>132</v>
+      </c>
+      <c r="I161" t="s">
+        <v>99</v>
+      </c>
+      <c r="L161" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M161" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A162">
+        <v>161</v>
+      </c>
+      <c r="B162">
+        <v>161</v>
+      </c>
+      <c r="C162" t="s">
         <v>106</v>
       </c>
-      <c r="F161" t="s">
-        <v>81</v>
-      </c>
-      <c r="G161" t="s">
-        <v>84</v>
-      </c>
-      <c r="H161" t="s">
+      <c r="D162" s="1">
+        <v>43888</v>
+      </c>
+      <c r="F162" t="s">
+        <v>81</v>
+      </c>
+      <c r="G162" t="s">
+        <v>84</v>
+      </c>
+      <c r="H162" t="s">
         <v>278</v>
       </c>
-      <c r="I161" t="s">
+      <c r="I162" t="s">
         <v>363</v>
       </c>
+      <c r="L162" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M162" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A163">
+        <v>162</v>
+      </c>
+      <c r="B163">
+        <v>162</v>
+      </c>
+      <c r="C163" t="s">
+        <v>106</v>
+      </c>
+      <c r="D163" s="1">
+        <v>43888</v>
+      </c>
+      <c r="F163" t="s">
+        <v>81</v>
+      </c>
+      <c r="G163" t="s">
+        <v>79</v>
+      </c>
+      <c r="H163" t="s">
+        <v>364</v>
+      </c>
+      <c r="I163" t="s">
+        <v>365</v>
+      </c>
+      <c r="L163" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M163" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A164">
+        <v>163</v>
+      </c>
+      <c r="B164">
+        <v>163</v>
+      </c>
+      <c r="C164" t="s">
+        <v>12</v>
+      </c>
+      <c r="D164" s="1">
+        <v>43888</v>
+      </c>
+      <c r="F164" t="s">
+        <v>81</v>
+      </c>
+      <c r="G164" t="s">
+        <v>84</v>
+      </c>
+      <c r="H164" t="s">
+        <v>366</v>
+      </c>
+      <c r="I164" t="s">
+        <v>367</v>
+      </c>
+      <c r="L164" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M164" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A165">
+        <v>164</v>
+      </c>
+      <c r="B165">
+        <v>164</v>
+      </c>
+      <c r="C165" t="s">
+        <v>12</v>
+      </c>
+      <c r="D165" s="1">
+        <v>43888</v>
+      </c>
+      <c r="F165" t="s">
+        <v>81</v>
+      </c>
+      <c r="G165" t="s">
+        <v>79</v>
+      </c>
+      <c r="H165" t="s">
+        <v>214</v>
+      </c>
+      <c r="I165" t="s">
+        <v>283</v>
+      </c>
+      <c r="L165" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M165" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A166">
+        <v>165</v>
+      </c>
+      <c r="B166">
+        <v>165</v>
+      </c>
+      <c r="C166" t="s">
+        <v>91</v>
+      </c>
+      <c r="D166" s="1">
+        <v>43888</v>
+      </c>
+      <c r="F166" t="s">
+        <v>165</v>
+      </c>
+      <c r="H166" t="s">
+        <v>368</v>
+      </c>
+      <c r="L166" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M166" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A167">
+        <v>166</v>
+      </c>
+      <c r="B167">
+        <v>166</v>
+      </c>
+      <c r="C167" t="s">
+        <v>34</v>
+      </c>
+      <c r="D167" s="1">
+        <v>43889</v>
+      </c>
+      <c r="F167" t="s">
+        <v>81</v>
+      </c>
+      <c r="G167" t="s">
+        <v>84</v>
+      </c>
+      <c r="H167" t="s">
+        <v>131</v>
+      </c>
+      <c r="I167" t="s">
+        <v>344</v>
+      </c>
+      <c r="L167" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M167" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A168">
+        <v>167</v>
+      </c>
+      <c r="B168">
+        <v>167</v>
+      </c>
+      <c r="C168" t="s">
+        <v>18</v>
+      </c>
+      <c r="D168" s="1">
+        <v>43889</v>
+      </c>
+      <c r="F168" t="s">
+        <v>81</v>
+      </c>
+      <c r="G168" t="s">
+        <v>84</v>
+      </c>
+      <c r="H168" t="s">
+        <v>131</v>
+      </c>
+      <c r="I168" t="s">
+        <v>344</v>
+      </c>
+      <c r="L168" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M168" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A169">
+        <v>168</v>
+      </c>
+      <c r="B169">
+        <v>168</v>
+      </c>
+      <c r="C169" t="s">
+        <v>17</v>
+      </c>
+      <c r="D169" s="1">
+        <v>43889</v>
+      </c>
+      <c r="F169" t="s">
+        <v>81</v>
+      </c>
+      <c r="G169" t="s">
+        <v>84</v>
+      </c>
+      <c r="H169" t="s">
+        <v>369</v>
+      </c>
+      <c r="I169" t="s">
+        <v>370</v>
+      </c>
+      <c r="L169" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M169" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A170">
+        <v>169</v>
+      </c>
+      <c r="B170">
+        <v>169</v>
+      </c>
+      <c r="C170" t="s">
+        <v>271</v>
+      </c>
+      <c r="D170" s="1">
+        <v>43889</v>
+      </c>
+      <c r="F170" t="s">
+        <v>81</v>
+      </c>
+      <c r="G170" t="s">
+        <v>84</v>
+      </c>
+      <c r="H170" t="s">
+        <v>369</v>
+      </c>
+      <c r="I170" t="s">
+        <v>370</v>
+      </c>
+      <c r="L170" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M170" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A171">
+        <v>170</v>
+      </c>
+      <c r="B171">
+        <v>170</v>
+      </c>
+      <c r="C171" t="s">
+        <v>223</v>
+      </c>
+      <c r="D171" s="1">
+        <v>43889</v>
+      </c>
+      <c r="F171" t="s">
+        <v>81</v>
+      </c>
+      <c r="G171" t="s">
+        <v>84</v>
+      </c>
+      <c r="H171" t="s">
+        <v>377</v>
+      </c>
+      <c r="I171" t="s">
+        <v>378</v>
+      </c>
+      <c r="L171" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M171" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A172">
+        <v>171</v>
+      </c>
+      <c r="B172">
+        <v>171</v>
+      </c>
+      <c r="C172" t="s">
+        <v>39</v>
+      </c>
+      <c r="D172" s="1">
+        <v>43890</v>
+      </c>
+      <c r="F172" t="s">
+        <v>81</v>
+      </c>
+      <c r="G172" t="s">
+        <v>84</v>
+      </c>
+      <c r="H172" t="s">
+        <v>371</v>
+      </c>
+      <c r="I172" t="s">
+        <v>372</v>
+      </c>
+      <c r="L172" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M172" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A173">
+        <v>172</v>
+      </c>
+      <c r="B173">
+        <v>172</v>
+      </c>
+      <c r="C173" t="s">
+        <v>39</v>
+      </c>
+      <c r="D173" s="1">
+        <v>43890</v>
+      </c>
+      <c r="F173" t="s">
+        <v>81</v>
+      </c>
+      <c r="G173" t="s">
+        <v>79</v>
+      </c>
+      <c r="H173" t="s">
+        <v>214</v>
+      </c>
+      <c r="I173" t="s">
+        <v>283</v>
+      </c>
+      <c r="L173" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M173" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A174">
+        <v>173</v>
+      </c>
+      <c r="B174">
+        <v>173</v>
+      </c>
+      <c r="C174" t="s">
+        <v>223</v>
+      </c>
+      <c r="D174" s="1">
+        <v>43890</v>
+      </c>
+      <c r="F174" t="s">
+        <v>81</v>
+      </c>
+      <c r="G174" t="s">
+        <v>84</v>
+      </c>
+      <c r="H174" t="s">
+        <v>373</v>
+      </c>
+      <c r="I174" t="s">
+        <v>374</v>
+      </c>
+      <c r="L174" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M174" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A175">
+        <v>174</v>
+      </c>
+      <c r="B175">
+        <v>174</v>
+      </c>
+      <c r="C175" t="s">
+        <v>223</v>
+      </c>
+      <c r="D175" s="1">
+        <v>43890</v>
+      </c>
+      <c r="F175" t="s">
+        <v>81</v>
+      </c>
+      <c r="G175" t="s">
+        <v>79</v>
+      </c>
+      <c r="H175" t="s">
+        <v>375</v>
+      </c>
+      <c r="I175" t="s">
+        <v>376</v>
+      </c>
+      <c r="L175" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M175" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A176">
+        <v>175</v>
+      </c>
+      <c r="B176">
+        <v>175</v>
+      </c>
+      <c r="C176" t="s">
+        <v>379</v>
+      </c>
+      <c r="D176" s="1">
+        <v>43890</v>
+      </c>
+      <c r="F176" t="s">
+        <v>81</v>
+      </c>
+      <c r="G176" t="s">
+        <v>84</v>
+      </c>
+      <c r="H176" t="s">
+        <v>131</v>
+      </c>
+      <c r="I176" t="s">
+        <v>344</v>
+      </c>
+      <c r="L176" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M176" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A177">
+        <v>176</v>
+      </c>
+      <c r="B177">
+        <v>176</v>
+      </c>
+      <c r="L177" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M177" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A178">
+        <v>177</v>
+      </c>
+      <c r="B178">
+        <v>177</v>
+      </c>
+      <c r="L178" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M178" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A179">
+        <v>178</v>
+      </c>
+      <c r="B179">
+        <v>178</v>
+      </c>
+      <c r="L179" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M179" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A180">
+        <v>179</v>
+      </c>
+      <c r="B180">
+        <v>179</v>
+      </c>
+      <c r="L180" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M180" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A181">
+        <v>180</v>
+      </c>
+      <c r="B181">
+        <v>180</v>
+      </c>
+      <c r="L181" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M181" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A182">
+        <v>181</v>
+      </c>
+      <c r="B182">
+        <v>181</v>
+      </c>
+      <c r="L182" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M182" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A183">
+        <v>182</v>
+      </c>
+      <c r="B183">
+        <v>182</v>
+      </c>
+      <c r="L183" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M183" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A184">
+        <v>183</v>
+      </c>
+      <c r="B184">
+        <v>183</v>
+      </c>
+      <c r="L184" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M184" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A185">
+        <v>184</v>
+      </c>
+      <c r="B185">
+        <v>184</v>
+      </c>
+      <c r="L185" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M185" s="1">
+        <v>43911</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A186">
+        <v>185</v>
+      </c>
+      <c r="B186">
+        <v>185</v>
+      </c>
+      <c r="L186" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M186" s="1">
+        <v>43911</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C122" xr:uid="{FEBE9123-A6FD-4349-BCC9-7DAEDCC15514}"/>
+  <autoFilter ref="C1:C123" xr:uid="{FEBE9123-A6FD-4349-BCC9-7DAEDCC15514}"/>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" xr:uid="{3C16743E-FB96-4E1A-AB85-5741C5C4837D}"/>
     <hyperlink ref="L3" r:id="rId2" xr:uid="{DCA54411-2475-41B6-9A87-99C3183173C6}"/>
@@ -6583,147 +7274,175 @@
     <hyperlink ref="L22" r:id="rId17" xr:uid="{3E8DF073-6CDA-487D-8FCF-9A2227382FCF}"/>
     <hyperlink ref="L17" r:id="rId18" xr:uid="{368BC015-78F8-4900-BF9D-3696F455A664}"/>
     <hyperlink ref="L18:L20" r:id="rId19" display="https://www.aljazeera.com/news/2020/01/timeline-china-coronavirus-spread-200126061554884.html" xr:uid="{5D786720-418A-41E3-86DA-F0ACF0A4CD27}"/>
-    <hyperlink ref="L23" r:id="rId20" xr:uid="{A3FE499D-BACD-43E8-9520-03A26BDD9DFA}"/>
-    <hyperlink ref="L24" r:id="rId21" xr:uid="{1D445D0C-2628-4734-BA96-9F93ADD15221}"/>
-    <hyperlink ref="L25" r:id="rId22" xr:uid="{724B156A-BA9A-41D7-BA6F-42F1A5B55B9C}"/>
-    <hyperlink ref="L26" r:id="rId23" xr:uid="{EF5531D8-D9DE-47F2-8F73-B6306AD4ED4E}"/>
-    <hyperlink ref="L27" r:id="rId24" xr:uid="{BB7ED08A-D40F-43AE-AE2F-31AD408DD5DA}"/>
-    <hyperlink ref="L28" r:id="rId25" xr:uid="{64969F41-CEC6-4488-84B5-7B077AF7B0D0}"/>
-    <hyperlink ref="L29" r:id="rId26" xr:uid="{B848F6AE-A7F3-43E8-82ED-2C7CF44CE1FE}"/>
-    <hyperlink ref="L30" r:id="rId27" xr:uid="{1BCBB0D9-0245-40C7-92B9-A26777719FC9}"/>
-    <hyperlink ref="L31" r:id="rId28" xr:uid="{A4C4CAD9-4C5B-4E96-9880-B44A33DA57D3}"/>
-    <hyperlink ref="L32" r:id="rId29" xr:uid="{606953EF-BD46-4D79-85EE-D33948099C1A}"/>
-    <hyperlink ref="L33" r:id="rId30" xr:uid="{C076FCC1-CC01-4B42-A97B-8C08A4D79D9A}"/>
-    <hyperlink ref="L34" r:id="rId31" xr:uid="{5B25595D-3CF0-4FB3-86FF-AE3DCA531396}"/>
-    <hyperlink ref="L35" r:id="rId32" xr:uid="{0893CF54-FEA5-44B5-863D-D173B528811E}"/>
-    <hyperlink ref="L36" r:id="rId33" xr:uid="{1846C43C-3397-4A95-BF9A-FF5DB964701E}"/>
-    <hyperlink ref="L37" r:id="rId34" xr:uid="{DBCA2D82-E818-4B29-8E05-DE72B02CB836}"/>
-    <hyperlink ref="L38" r:id="rId35" xr:uid="{D20FA874-C2DE-4074-ABA3-0BAD079F5204}"/>
-    <hyperlink ref="L39" r:id="rId36" xr:uid="{9AB19D0A-D0DE-48C3-9217-90E8557F96C3}"/>
-    <hyperlink ref="L40" r:id="rId37" xr:uid="{2859B84C-BADE-46BB-B99F-798697C7B12C}"/>
-    <hyperlink ref="L41" r:id="rId38" xr:uid="{1578FAD3-231A-4EE6-BA27-D420380601FC}"/>
-    <hyperlink ref="L42" r:id="rId39" xr:uid="{2FE05711-A7BC-4833-ABF1-E96246EABE80}"/>
-    <hyperlink ref="L43" r:id="rId40" xr:uid="{E6EE7F0C-B517-43B6-9E4E-876579DC87B0}"/>
-    <hyperlink ref="L44" r:id="rId41" xr:uid="{DB9C6FD0-E0FB-4099-B4E7-6B587ADA397B}"/>
-    <hyperlink ref="L45" r:id="rId42" xr:uid="{C9BABEB3-32DE-43A3-A707-3C8447B591F1}"/>
-    <hyperlink ref="L46" r:id="rId43" xr:uid="{30AFC5E4-787D-46E8-A31A-0CAA51D3D5DC}"/>
-    <hyperlink ref="L47" r:id="rId44" xr:uid="{00870976-7C06-4E52-A502-35DF8CFA42F3}"/>
-    <hyperlink ref="L48" r:id="rId45" xr:uid="{DA8D03FD-30FB-4019-886F-CB744E85694A}"/>
-    <hyperlink ref="L49" r:id="rId46" xr:uid="{23582090-EA83-4FB2-94C6-2EC749F91FE1}"/>
-    <hyperlink ref="L50" r:id="rId47" xr:uid="{EE569A5D-4C8F-4A5D-8478-9F29FD668AB5}"/>
-    <hyperlink ref="L51" r:id="rId48" xr:uid="{DCE06ED8-D784-42A2-A7E0-1DB7C34236A6}"/>
-    <hyperlink ref="L52" r:id="rId49" xr:uid="{A6679CCD-4F8B-4378-BC2B-CCAB238B1F83}"/>
-    <hyperlink ref="L53" r:id="rId50" xr:uid="{D3BB259B-4F45-4DF4-972A-010C3A1A020F}"/>
-    <hyperlink ref="L54" r:id="rId51" xr:uid="{AA6CDFCA-0F62-4629-8E12-82878C98604F}"/>
-    <hyperlink ref="L55" r:id="rId52" xr:uid="{474425BC-BC6C-4337-AB19-765C2BB9E1CC}"/>
-    <hyperlink ref="L56" r:id="rId53" xr:uid="{3F6E72F0-2EF3-4FC3-BA3D-A665B2525BA6}"/>
-    <hyperlink ref="L57" r:id="rId54" xr:uid="{FFE58A0A-B685-4267-A35A-A96FAE425585}"/>
-    <hyperlink ref="L58" r:id="rId55" xr:uid="{09B8B4B1-E9F6-4850-B2F9-9B95C56D0446}"/>
-    <hyperlink ref="L59" r:id="rId56" xr:uid="{307C1FF0-EC6E-4853-A8AC-A701736B64EA}"/>
-    <hyperlink ref="L60" r:id="rId57" xr:uid="{5C830347-0BE0-4D8A-A2EF-7452505571E9}"/>
-    <hyperlink ref="L61" r:id="rId58" xr:uid="{6432EC6A-1C30-43BA-8ECB-63619A454214}"/>
-    <hyperlink ref="L62" r:id="rId59" xr:uid="{951BB29A-7665-444B-8E13-6EA02F77CF9D}"/>
-    <hyperlink ref="L63" r:id="rId60" xr:uid="{36B4E049-03C6-45CA-8E56-C4CA6EDB6D61}"/>
-    <hyperlink ref="L64" r:id="rId61" xr:uid="{9992ACDB-FBD6-4682-A26B-CC173638690B}"/>
-    <hyperlink ref="L65" r:id="rId62" xr:uid="{6C814A5F-926B-4806-9E5A-185F9795A8AD}"/>
-    <hyperlink ref="L66" r:id="rId63" xr:uid="{DA55E0C7-50A9-4BB1-8394-90612CC2EC37}"/>
-    <hyperlink ref="L67" r:id="rId64" xr:uid="{E9F40236-CD4F-4E8D-BF5E-7E833049C1C6}"/>
-    <hyperlink ref="L68" r:id="rId65" xr:uid="{FBEB110C-791C-4C6B-A3A5-E24FF944FE2D}"/>
-    <hyperlink ref="L69" r:id="rId66" xr:uid="{4A6F8F26-F3B0-48EB-9E36-CD86CAC93915}"/>
-    <hyperlink ref="L70" r:id="rId67" xr:uid="{A66781B2-1FC5-498E-A91F-F189AB5E7968}"/>
-    <hyperlink ref="L71" r:id="rId68" xr:uid="{38E34C05-633C-44C6-9662-4750E60484AE}"/>
-    <hyperlink ref="L72" r:id="rId69" xr:uid="{FE0295E9-94D5-4DC7-AF98-6DA47217D7D0}"/>
-    <hyperlink ref="L73" r:id="rId70" xr:uid="{06DF2F83-88A6-449C-B28F-3C134D41C558}"/>
-    <hyperlink ref="L74" r:id="rId71" xr:uid="{5485D62C-C3F2-41EA-BF41-6B797055A35F}"/>
-    <hyperlink ref="L75" r:id="rId72" xr:uid="{6ADD31F5-FE76-49D4-8104-A02C158B84DF}"/>
-    <hyperlink ref="L76" r:id="rId73" xr:uid="{986EDA82-CAF1-4046-81CD-E55192043A26}"/>
-    <hyperlink ref="L77" r:id="rId74" xr:uid="{112BA9B7-3582-4586-86FF-E513B1FD774D}"/>
-    <hyperlink ref="L78" r:id="rId75" xr:uid="{B8DDB6C2-CF59-4F55-A128-8FC460E0CEE4}"/>
-    <hyperlink ref="L79" r:id="rId76" xr:uid="{CE709831-306F-4B47-A1CD-C27F1D04266F}"/>
-    <hyperlink ref="L80" r:id="rId77" xr:uid="{4C54F905-D8C6-4B2E-8943-C9B27EB818A2}"/>
-    <hyperlink ref="L81" r:id="rId78" xr:uid="{FFFF7BD7-401A-4156-8C5E-EB09F00B1829}"/>
-    <hyperlink ref="L82" r:id="rId79" xr:uid="{E02DA36F-0EED-4783-A458-6F024A0C5543}"/>
-    <hyperlink ref="L83" r:id="rId80" xr:uid="{6483773C-B24F-4AE7-9601-2A15B49F365E}"/>
-    <hyperlink ref="L84" r:id="rId81" xr:uid="{4500A3F1-F90F-4739-A80F-3D6FEB38E5A2}"/>
-    <hyperlink ref="L85" r:id="rId82" xr:uid="{868D9225-8DA2-4B5F-956F-4808E55C17AA}"/>
-    <hyperlink ref="L86" r:id="rId83" xr:uid="{E0AFC9CD-BB4B-4938-ACA6-12168676A5C0}"/>
-    <hyperlink ref="L87" r:id="rId84" xr:uid="{2DA94908-DCCD-4CEB-B28C-B86F3E06ED85}"/>
-    <hyperlink ref="L88" r:id="rId85" xr:uid="{046B8DCE-5312-4B2E-8ECA-E6F1BC3751FE}"/>
-    <hyperlink ref="L89" r:id="rId86" xr:uid="{68D56F9F-858B-4D41-A3A9-F68435AA3FF6}"/>
-    <hyperlink ref="L90" r:id="rId87" xr:uid="{D9D1261A-7E7B-4183-9CAA-DA87F1218712}"/>
-    <hyperlink ref="L91" r:id="rId88" xr:uid="{10036F27-B0EC-4B69-B763-19970A708266}"/>
-    <hyperlink ref="L92" r:id="rId89" xr:uid="{270954E3-7949-4AD1-B28E-D2F7949B8005}"/>
-    <hyperlink ref="L93" r:id="rId90" xr:uid="{4CFF0B56-A457-4C16-9DA1-0777017A1F00}"/>
-    <hyperlink ref="L94" r:id="rId91" xr:uid="{2F0B761A-9BFC-4CE2-8E83-CB3B0CC8CF36}"/>
-    <hyperlink ref="L95" r:id="rId92" xr:uid="{794E7341-BDE7-4388-B6C7-4373A8A6F8CC}"/>
-    <hyperlink ref="L96" r:id="rId93" xr:uid="{32FB6B00-3E61-46F4-8029-FE3343BBF62A}"/>
-    <hyperlink ref="L97" r:id="rId94" xr:uid="{AF869895-2547-4852-9F56-6CFD4F8AB79C}"/>
-    <hyperlink ref="L98" r:id="rId95" xr:uid="{330FEBC3-7DCE-43F0-8F5E-7F2C40828DD0}"/>
-    <hyperlink ref="L99" r:id="rId96" xr:uid="{7C25A172-BC98-4C65-A291-AF7BDCEEE5AD}"/>
-    <hyperlink ref="L101" r:id="rId97" xr:uid="{793884E6-93B1-4BB5-B34D-AB9248403DDC}"/>
-    <hyperlink ref="L102" r:id="rId98" xr:uid="{98F2051D-5B52-4C88-B8F1-ABAD7CC14FE0}"/>
-    <hyperlink ref="L103" r:id="rId99" xr:uid="{79778209-B43C-4643-9559-EFA41393F18D}"/>
-    <hyperlink ref="L104" r:id="rId100" xr:uid="{3AD16CFE-849E-4915-B2F1-F609ACB95F17}"/>
-    <hyperlink ref="L105" r:id="rId101" xr:uid="{FF097E96-0A1B-4A1F-AEC7-1386EE177420}"/>
-    <hyperlink ref="L106" r:id="rId102" xr:uid="{53701C6C-E479-46C1-8BEF-9AAB7578731B}"/>
-    <hyperlink ref="L107" r:id="rId103" xr:uid="{2ED19BC5-B2A2-4D61-BE98-9162D61DF7AE}"/>
-    <hyperlink ref="L108" r:id="rId104" xr:uid="{8E9A3B67-7795-4474-8769-E54FD02DFC27}"/>
-    <hyperlink ref="L109" r:id="rId105" xr:uid="{B8849DCA-9EED-45E3-A751-C26642989720}"/>
-    <hyperlink ref="L110" r:id="rId106" xr:uid="{40F8281C-C803-45C1-811B-65CBBDB78D90}"/>
-    <hyperlink ref="L100" r:id="rId107" xr:uid="{AE0B97BA-49D3-45F3-8DB9-053C0932EA25}"/>
-    <hyperlink ref="L111" r:id="rId108" xr:uid="{4D167150-B5BC-40E5-8ACA-C5AEC3AF2231}"/>
-    <hyperlink ref="L112" r:id="rId109" xr:uid="{081575A8-D3B0-4E10-96A5-E13D70CBE231}"/>
-    <hyperlink ref="L113" r:id="rId110" xr:uid="{D4A5F1EC-A182-42BE-B826-53D6B9C586CD}"/>
-    <hyperlink ref="L114" r:id="rId111" xr:uid="{6806EB61-F3E7-438C-AF1A-640F1EA4215A}"/>
-    <hyperlink ref="L115" r:id="rId112" xr:uid="{BD66E2C5-E047-439C-98E7-2894B349A7D9}"/>
-    <hyperlink ref="L116" r:id="rId113" xr:uid="{C137EC48-4154-47EC-AEE9-5D916853DFF3}"/>
-    <hyperlink ref="L117" r:id="rId114" xr:uid="{8B2D3BAF-9BF4-4E49-8555-42F3325A9044}"/>
-    <hyperlink ref="L118" r:id="rId115" xr:uid="{645D1F3E-E24E-4D05-8459-50D11F1B1362}"/>
-    <hyperlink ref="L119" r:id="rId116" xr:uid="{395C4C2C-3FBE-4D53-892F-F4F2347E36FD}"/>
-    <hyperlink ref="L120" r:id="rId117" xr:uid="{4B3E987A-E57D-4AE4-B395-ADCBA3191132}"/>
-    <hyperlink ref="L121" r:id="rId118" xr:uid="{95A5A889-701B-4545-9A3E-6F5EE9C941E0}"/>
-    <hyperlink ref="L122" r:id="rId119" xr:uid="{EC3FAE8D-9875-497C-8E55-C2215CC5B0B0}"/>
-    <hyperlink ref="L123" r:id="rId120" xr:uid="{7BE90F72-445E-454E-B4EB-27029F098390}"/>
-    <hyperlink ref="L124" r:id="rId121" xr:uid="{4CB22FBB-B5A5-4505-9348-1B681A4CCD2F}"/>
-    <hyperlink ref="L125" r:id="rId122" xr:uid="{DCE456CA-44BE-41B3-9FDE-6CB687711836}"/>
-    <hyperlink ref="L126" r:id="rId123" xr:uid="{EA3F0089-8880-454F-B098-D7E2E9E56A02}"/>
-    <hyperlink ref="L127" r:id="rId124" xr:uid="{CDF2C053-6DC6-489E-B0B8-1F2BB5321BB6}"/>
-    <hyperlink ref="L128" r:id="rId125" xr:uid="{16EC32C5-5C0F-4A0C-9C4D-8B34BA83D6C8}"/>
-    <hyperlink ref="L129" r:id="rId126" xr:uid="{D60B803A-743B-4203-9EB8-9E9070882D35}"/>
-    <hyperlink ref="L130" r:id="rId127" xr:uid="{E43CC7C6-B9FA-4408-ABD3-229DA76D52BA}"/>
-    <hyperlink ref="L131" r:id="rId128" xr:uid="{411167BC-0EEB-47C3-9580-F7B31B4C6DA5}"/>
-    <hyperlink ref="L132" r:id="rId129" xr:uid="{07A16AA3-F9AE-47BE-A85D-52A4C83C3C46}"/>
-    <hyperlink ref="L133" r:id="rId130" xr:uid="{A31B1BFE-7C91-4A21-898F-827AB12B4DB9}"/>
-    <hyperlink ref="L134" r:id="rId131" xr:uid="{82862421-0C7E-4B77-90E1-498870B39DA4}"/>
-    <hyperlink ref="L135" r:id="rId132" xr:uid="{805690AE-D15F-4D1E-9B40-A5861E507294}"/>
-    <hyperlink ref="L136" r:id="rId133" xr:uid="{B216D342-090B-417B-B663-C80CF196EF97}"/>
-    <hyperlink ref="L137" r:id="rId134" xr:uid="{2DD7BC89-BD05-478B-8CF3-FD7D5454154A}"/>
-    <hyperlink ref="L138" r:id="rId135" xr:uid="{AAAC16E4-D7C5-44B0-B3BB-35D1395FCDAF}"/>
-    <hyperlink ref="L139" r:id="rId136" xr:uid="{063A5232-D399-4340-8DDE-FB7D1F68BBE2}"/>
-    <hyperlink ref="L140" r:id="rId137" xr:uid="{A1E50341-6B11-4760-B319-F13BCA89F11E}"/>
-    <hyperlink ref="L141" r:id="rId138" xr:uid="{874745CF-CFBD-4282-8DF1-A56B01093359}"/>
-    <hyperlink ref="L142" r:id="rId139" xr:uid="{7AAF33C2-BF47-4607-AB21-A287FF6260D0}"/>
-    <hyperlink ref="L143" r:id="rId140" xr:uid="{33CA3AE9-4018-44E4-B1F9-640415F092DC}"/>
-    <hyperlink ref="L146" r:id="rId141" xr:uid="{4E56EE8C-7B60-4916-888B-47B24752392D}"/>
-    <hyperlink ref="L147" r:id="rId142" xr:uid="{02ACD3AA-6D5E-48A5-B841-8D58CB3E690B}"/>
-    <hyperlink ref="L148" r:id="rId143" xr:uid="{E45867E8-7130-45C0-A634-2A75E347E531}"/>
-    <hyperlink ref="L149" r:id="rId144" xr:uid="{28D0A458-F098-43AB-8FE5-A67A34DD0BC1}"/>
-    <hyperlink ref="L144" r:id="rId145" xr:uid="{7BC68CF8-5A01-47DC-852E-3A474B71A4BD}"/>
-    <hyperlink ref="L145" r:id="rId146" xr:uid="{D980D1A9-4124-46CB-8A21-1075F5C89262}"/>
-    <hyperlink ref="L150" r:id="rId147" xr:uid="{2EE1C1D9-60C6-4933-90B8-FF8D6DB54BE0}"/>
-    <hyperlink ref="L151" r:id="rId148" xr:uid="{7E1F82D2-1487-42CA-8F49-8840CA00D9BD}"/>
-    <hyperlink ref="L152" r:id="rId149" xr:uid="{E9675B85-CCCC-41EC-A374-8B0EEB687ABF}"/>
-    <hyperlink ref="L153" r:id="rId150" xr:uid="{E8CD8B29-C864-43B7-BF17-29C62184BEA9}"/>
-    <hyperlink ref="L154" r:id="rId151" xr:uid="{B95D0080-64D2-4BCA-93D4-1F546B829CEF}"/>
-    <hyperlink ref="L155" r:id="rId152" xr:uid="{F36468A9-7021-46EC-AE95-EB51D2206B9A}"/>
-    <hyperlink ref="L156" r:id="rId153" xr:uid="{7AC1AF03-79E4-4622-B8E2-C18330DC3F9A}"/>
-    <hyperlink ref="L157" r:id="rId154" xr:uid="{609C026B-4ACB-4FF6-AC60-7FD4914093B9}"/>
-    <hyperlink ref="L158" r:id="rId155" xr:uid="{0F4685AB-B355-4755-BF99-0D9A14723E3C}"/>
+    <hyperlink ref="L24" r:id="rId20" xr:uid="{1D445D0C-2628-4734-BA96-9F93ADD15221}"/>
+    <hyperlink ref="L25" r:id="rId21" xr:uid="{724B156A-BA9A-41D7-BA6F-42F1A5B55B9C}"/>
+    <hyperlink ref="L26" r:id="rId22" xr:uid="{EF5531D8-D9DE-47F2-8F73-B6306AD4ED4E}"/>
+    <hyperlink ref="L27" r:id="rId23" xr:uid="{BB7ED08A-D40F-43AE-AE2F-31AD408DD5DA}"/>
+    <hyperlink ref="L28" r:id="rId24" xr:uid="{64969F41-CEC6-4488-84B5-7B077AF7B0D0}"/>
+    <hyperlink ref="L29" r:id="rId25" xr:uid="{B848F6AE-A7F3-43E8-82ED-2C7CF44CE1FE}"/>
+    <hyperlink ref="L30" r:id="rId26" xr:uid="{1BCBB0D9-0245-40C7-92B9-A26777719FC9}"/>
+    <hyperlink ref="L31" r:id="rId27" xr:uid="{A4C4CAD9-4C5B-4E96-9880-B44A33DA57D3}"/>
+    <hyperlink ref="L32" r:id="rId28" xr:uid="{606953EF-BD46-4D79-85EE-D33948099C1A}"/>
+    <hyperlink ref="L33" r:id="rId29" xr:uid="{C076FCC1-CC01-4B42-A97B-8C08A4D79D9A}"/>
+    <hyperlink ref="L34" r:id="rId30" xr:uid="{5B25595D-3CF0-4FB3-86FF-AE3DCA531396}"/>
+    <hyperlink ref="L35" r:id="rId31" xr:uid="{0893CF54-FEA5-44B5-863D-D173B528811E}"/>
+    <hyperlink ref="L36" r:id="rId32" xr:uid="{1846C43C-3397-4A95-BF9A-FF5DB964701E}"/>
+    <hyperlink ref="L37" r:id="rId33" xr:uid="{DBCA2D82-E818-4B29-8E05-DE72B02CB836}"/>
+    <hyperlink ref="L38" r:id="rId34" xr:uid="{D20FA874-C2DE-4074-ABA3-0BAD079F5204}"/>
+    <hyperlink ref="L39" r:id="rId35" xr:uid="{9AB19D0A-D0DE-48C3-9217-90E8557F96C3}"/>
+    <hyperlink ref="L40" r:id="rId36" xr:uid="{2859B84C-BADE-46BB-B99F-798697C7B12C}"/>
+    <hyperlink ref="L41" r:id="rId37" xr:uid="{1578FAD3-231A-4EE6-BA27-D420380601FC}"/>
+    <hyperlink ref="L42" r:id="rId38" xr:uid="{2FE05711-A7BC-4833-ABF1-E96246EABE80}"/>
+    <hyperlink ref="L43" r:id="rId39" xr:uid="{E6EE7F0C-B517-43B6-9E4E-876579DC87B0}"/>
+    <hyperlink ref="L44" r:id="rId40" xr:uid="{DB9C6FD0-E0FB-4099-B4E7-6B587ADA397B}"/>
+    <hyperlink ref="L45" r:id="rId41" xr:uid="{C9BABEB3-32DE-43A3-A707-3C8447B591F1}"/>
+    <hyperlink ref="L46" r:id="rId42" xr:uid="{30AFC5E4-787D-46E8-A31A-0CAA51D3D5DC}"/>
+    <hyperlink ref="L47" r:id="rId43" xr:uid="{00870976-7C06-4E52-A502-35DF8CFA42F3}"/>
+    <hyperlink ref="L48" r:id="rId44" xr:uid="{DA8D03FD-30FB-4019-886F-CB744E85694A}"/>
+    <hyperlink ref="L49" r:id="rId45" xr:uid="{23582090-EA83-4FB2-94C6-2EC749F91FE1}"/>
+    <hyperlink ref="L50" r:id="rId46" xr:uid="{EE569A5D-4C8F-4A5D-8478-9F29FD668AB5}"/>
+    <hyperlink ref="L51" r:id="rId47" xr:uid="{DCE06ED8-D784-42A2-A7E0-1DB7C34236A6}"/>
+    <hyperlink ref="L52" r:id="rId48" xr:uid="{A6679CCD-4F8B-4378-BC2B-CCAB238B1F83}"/>
+    <hyperlink ref="L53" r:id="rId49" xr:uid="{D3BB259B-4F45-4DF4-972A-010C3A1A020F}"/>
+    <hyperlink ref="L54" r:id="rId50" xr:uid="{AA6CDFCA-0F62-4629-8E12-82878C98604F}"/>
+    <hyperlink ref="L55" r:id="rId51" xr:uid="{474425BC-BC6C-4337-AB19-765C2BB9E1CC}"/>
+    <hyperlink ref="L56" r:id="rId52" xr:uid="{3F6E72F0-2EF3-4FC3-BA3D-A665B2525BA6}"/>
+    <hyperlink ref="L57" r:id="rId53" xr:uid="{FFE58A0A-B685-4267-A35A-A96FAE425585}"/>
+    <hyperlink ref="L58" r:id="rId54" xr:uid="{09B8B4B1-E9F6-4850-B2F9-9B95C56D0446}"/>
+    <hyperlink ref="L59" r:id="rId55" xr:uid="{307C1FF0-EC6E-4853-A8AC-A701736B64EA}"/>
+    <hyperlink ref="L60" r:id="rId56" xr:uid="{5C830347-0BE0-4D8A-A2EF-7452505571E9}"/>
+    <hyperlink ref="L61" r:id="rId57" xr:uid="{6432EC6A-1C30-43BA-8ECB-63619A454214}"/>
+    <hyperlink ref="L62" r:id="rId58" xr:uid="{951BB29A-7665-444B-8E13-6EA02F77CF9D}"/>
+    <hyperlink ref="L63" r:id="rId59" xr:uid="{36B4E049-03C6-45CA-8E56-C4CA6EDB6D61}"/>
+    <hyperlink ref="L64" r:id="rId60" xr:uid="{9992ACDB-FBD6-4682-A26B-CC173638690B}"/>
+    <hyperlink ref="L65" r:id="rId61" xr:uid="{6C814A5F-926B-4806-9E5A-185F9795A8AD}"/>
+    <hyperlink ref="L66" r:id="rId62" xr:uid="{DA55E0C7-50A9-4BB1-8394-90612CC2EC37}"/>
+    <hyperlink ref="L67" r:id="rId63" xr:uid="{E9F40236-CD4F-4E8D-BF5E-7E833049C1C6}"/>
+    <hyperlink ref="L68" r:id="rId64" xr:uid="{FBEB110C-791C-4C6B-A3A5-E24FF944FE2D}"/>
+    <hyperlink ref="L69" r:id="rId65" xr:uid="{4A6F8F26-F3B0-48EB-9E36-CD86CAC93915}"/>
+    <hyperlink ref="L70" r:id="rId66" xr:uid="{A66781B2-1FC5-498E-A91F-F189AB5E7968}"/>
+    <hyperlink ref="L71" r:id="rId67" xr:uid="{38E34C05-633C-44C6-9662-4750E60484AE}"/>
+    <hyperlink ref="L72" r:id="rId68" xr:uid="{FE0295E9-94D5-4DC7-AF98-6DA47217D7D0}"/>
+    <hyperlink ref="L73" r:id="rId69" xr:uid="{06DF2F83-88A6-449C-B28F-3C134D41C558}"/>
+    <hyperlink ref="L74" r:id="rId70" xr:uid="{5485D62C-C3F2-41EA-BF41-6B797055A35F}"/>
+    <hyperlink ref="L75" r:id="rId71" xr:uid="{6ADD31F5-FE76-49D4-8104-A02C158B84DF}"/>
+    <hyperlink ref="L76" r:id="rId72" xr:uid="{986EDA82-CAF1-4046-81CD-E55192043A26}"/>
+    <hyperlink ref="L77" r:id="rId73" xr:uid="{112BA9B7-3582-4586-86FF-E513B1FD774D}"/>
+    <hyperlink ref="L78" r:id="rId74" xr:uid="{B8DDB6C2-CF59-4F55-A128-8FC460E0CEE4}"/>
+    <hyperlink ref="L79" r:id="rId75" xr:uid="{CE709831-306F-4B47-A1CD-C27F1D04266F}"/>
+    <hyperlink ref="L80" r:id="rId76" xr:uid="{4C54F905-D8C6-4B2E-8943-C9B27EB818A2}"/>
+    <hyperlink ref="L81" r:id="rId77" xr:uid="{FFFF7BD7-401A-4156-8C5E-EB09F00B1829}"/>
+    <hyperlink ref="L82" r:id="rId78" xr:uid="{E02DA36F-0EED-4783-A458-6F024A0C5543}"/>
+    <hyperlink ref="L83" r:id="rId79" xr:uid="{6483773C-B24F-4AE7-9601-2A15B49F365E}"/>
+    <hyperlink ref="L84" r:id="rId80" xr:uid="{4500A3F1-F90F-4739-A80F-3D6FEB38E5A2}"/>
+    <hyperlink ref="L85" r:id="rId81" xr:uid="{868D9225-8DA2-4B5F-956F-4808E55C17AA}"/>
+    <hyperlink ref="L86" r:id="rId82" xr:uid="{E0AFC9CD-BB4B-4938-ACA6-12168676A5C0}"/>
+    <hyperlink ref="L87" r:id="rId83" xr:uid="{2DA94908-DCCD-4CEB-B28C-B86F3E06ED85}"/>
+    <hyperlink ref="L88" r:id="rId84" xr:uid="{046B8DCE-5312-4B2E-8ECA-E6F1BC3751FE}"/>
+    <hyperlink ref="L89" r:id="rId85" xr:uid="{68D56F9F-858B-4D41-A3A9-F68435AA3FF6}"/>
+    <hyperlink ref="L90" r:id="rId86" xr:uid="{D9D1261A-7E7B-4183-9CAA-DA87F1218712}"/>
+    <hyperlink ref="L91" r:id="rId87" xr:uid="{10036F27-B0EC-4B69-B763-19970A708266}"/>
+    <hyperlink ref="L92" r:id="rId88" xr:uid="{270954E3-7949-4AD1-B28E-D2F7949B8005}"/>
+    <hyperlink ref="L93" r:id="rId89" xr:uid="{4CFF0B56-A457-4C16-9DA1-0777017A1F00}"/>
+    <hyperlink ref="L94" r:id="rId90" xr:uid="{2F0B761A-9BFC-4CE2-8E83-CB3B0CC8CF36}"/>
+    <hyperlink ref="L95" r:id="rId91" xr:uid="{794E7341-BDE7-4388-B6C7-4373A8A6F8CC}"/>
+    <hyperlink ref="L96" r:id="rId92" xr:uid="{32FB6B00-3E61-46F4-8029-FE3343BBF62A}"/>
+    <hyperlink ref="L97" r:id="rId93" xr:uid="{AF869895-2547-4852-9F56-6CFD4F8AB79C}"/>
+    <hyperlink ref="L98" r:id="rId94" xr:uid="{330FEBC3-7DCE-43F0-8F5E-7F2C40828DD0}"/>
+    <hyperlink ref="L99" r:id="rId95" xr:uid="{7C25A172-BC98-4C65-A291-AF7BDCEEE5AD}"/>
+    <hyperlink ref="L101" r:id="rId96" xr:uid="{793884E6-93B1-4BB5-B34D-AB9248403DDC}"/>
+    <hyperlink ref="L102" r:id="rId97" xr:uid="{98F2051D-5B52-4C88-B8F1-ABAD7CC14FE0}"/>
+    <hyperlink ref="L103" r:id="rId98" xr:uid="{79778209-B43C-4643-9559-EFA41393F18D}"/>
+    <hyperlink ref="L104" r:id="rId99" xr:uid="{3AD16CFE-849E-4915-B2F1-F609ACB95F17}"/>
+    <hyperlink ref="L105" r:id="rId100" xr:uid="{FF097E96-0A1B-4A1F-AEC7-1386EE177420}"/>
+    <hyperlink ref="L106" r:id="rId101" xr:uid="{53701C6C-E479-46C1-8BEF-9AAB7578731B}"/>
+    <hyperlink ref="L107" r:id="rId102" xr:uid="{2ED19BC5-B2A2-4D61-BE98-9162D61DF7AE}"/>
+    <hyperlink ref="L108" r:id="rId103" xr:uid="{8E9A3B67-7795-4474-8769-E54FD02DFC27}"/>
+    <hyperlink ref="L109" r:id="rId104" xr:uid="{B8849DCA-9EED-45E3-A751-C26642989720}"/>
+    <hyperlink ref="L110" r:id="rId105" xr:uid="{40F8281C-C803-45C1-811B-65CBBDB78D90}"/>
+    <hyperlink ref="L100" r:id="rId106" xr:uid="{AE0B97BA-49D3-45F3-8DB9-053C0932EA25}"/>
+    <hyperlink ref="L111" r:id="rId107" xr:uid="{4D167150-B5BC-40E5-8ACA-C5AEC3AF2231}"/>
+    <hyperlink ref="L112" r:id="rId108" xr:uid="{081575A8-D3B0-4E10-96A5-E13D70CBE231}"/>
+    <hyperlink ref="L113" r:id="rId109" xr:uid="{D4A5F1EC-A182-42BE-B826-53D6B9C586CD}"/>
+    <hyperlink ref="L114" r:id="rId110" xr:uid="{6806EB61-F3E7-438C-AF1A-640F1EA4215A}"/>
+    <hyperlink ref="L115" r:id="rId111" xr:uid="{BD66E2C5-E047-439C-98E7-2894B349A7D9}"/>
+    <hyperlink ref="L116" r:id="rId112" xr:uid="{C137EC48-4154-47EC-AEE9-5D916853DFF3}"/>
+    <hyperlink ref="L117" r:id="rId113" xr:uid="{8B2D3BAF-9BF4-4E49-8555-42F3325A9044}"/>
+    <hyperlink ref="L118" r:id="rId114" xr:uid="{645D1F3E-E24E-4D05-8459-50D11F1B1362}"/>
+    <hyperlink ref="L119" r:id="rId115" xr:uid="{395C4C2C-3FBE-4D53-892F-F4F2347E36FD}"/>
+    <hyperlink ref="L120" r:id="rId116" xr:uid="{4B3E987A-E57D-4AE4-B395-ADCBA3191132}"/>
+    <hyperlink ref="L121" r:id="rId117" xr:uid="{95A5A889-701B-4545-9A3E-6F5EE9C941E0}"/>
+    <hyperlink ref="L123" r:id="rId118" xr:uid="{EC3FAE8D-9875-497C-8E55-C2215CC5B0B0}"/>
+    <hyperlink ref="L124" r:id="rId119" xr:uid="{7BE90F72-445E-454E-B4EB-27029F098390}"/>
+    <hyperlink ref="L125" r:id="rId120" xr:uid="{4CB22FBB-B5A5-4505-9348-1B681A4CCD2F}"/>
+    <hyperlink ref="L126" r:id="rId121" xr:uid="{DCE456CA-44BE-41B3-9FDE-6CB687711836}"/>
+    <hyperlink ref="L127" r:id="rId122" xr:uid="{EA3F0089-8880-454F-B098-D7E2E9E56A02}"/>
+    <hyperlink ref="L128" r:id="rId123" xr:uid="{CDF2C053-6DC6-489E-B0B8-1F2BB5321BB6}"/>
+    <hyperlink ref="L129" r:id="rId124" xr:uid="{16EC32C5-5C0F-4A0C-9C4D-8B34BA83D6C8}"/>
+    <hyperlink ref="L130" r:id="rId125" xr:uid="{D60B803A-743B-4203-9EB8-9E9070882D35}"/>
+    <hyperlink ref="L131" r:id="rId126" xr:uid="{E43CC7C6-B9FA-4408-ABD3-229DA76D52BA}"/>
+    <hyperlink ref="L132" r:id="rId127" xr:uid="{411167BC-0EEB-47C3-9580-F7B31B4C6DA5}"/>
+    <hyperlink ref="L133" r:id="rId128" xr:uid="{07A16AA3-F9AE-47BE-A85D-52A4C83C3C46}"/>
+    <hyperlink ref="L134" r:id="rId129" xr:uid="{A31B1BFE-7C91-4A21-898F-827AB12B4DB9}"/>
+    <hyperlink ref="L135" r:id="rId130" xr:uid="{82862421-0C7E-4B77-90E1-498870B39DA4}"/>
+    <hyperlink ref="L136" r:id="rId131" xr:uid="{805690AE-D15F-4D1E-9B40-A5861E507294}"/>
+    <hyperlink ref="L137" r:id="rId132" xr:uid="{B216D342-090B-417B-B663-C80CF196EF97}"/>
+    <hyperlink ref="L138" r:id="rId133" xr:uid="{2DD7BC89-BD05-478B-8CF3-FD7D5454154A}"/>
+    <hyperlink ref="L139" r:id="rId134" xr:uid="{AAAC16E4-D7C5-44B0-B3BB-35D1395FCDAF}"/>
+    <hyperlink ref="L140" r:id="rId135" xr:uid="{063A5232-D399-4340-8DDE-FB7D1F68BBE2}"/>
+    <hyperlink ref="L141" r:id="rId136" xr:uid="{A1E50341-6B11-4760-B319-F13BCA89F11E}"/>
+    <hyperlink ref="L142" r:id="rId137" xr:uid="{874745CF-CFBD-4282-8DF1-A56B01093359}"/>
+    <hyperlink ref="L143" r:id="rId138" xr:uid="{7AAF33C2-BF47-4607-AB21-A287FF6260D0}"/>
+    <hyperlink ref="L144" r:id="rId139" xr:uid="{33CA3AE9-4018-44E4-B1F9-640415F092DC}"/>
+    <hyperlink ref="L147" r:id="rId140" xr:uid="{4E56EE8C-7B60-4916-888B-47B24752392D}"/>
+    <hyperlink ref="L148" r:id="rId141" xr:uid="{02ACD3AA-6D5E-48A5-B841-8D58CB3E690B}"/>
+    <hyperlink ref="L149" r:id="rId142" xr:uid="{E45867E8-7130-45C0-A634-2A75E347E531}"/>
+    <hyperlink ref="L150" r:id="rId143" xr:uid="{28D0A458-F098-43AB-8FE5-A67A34DD0BC1}"/>
+    <hyperlink ref="L145" r:id="rId144" xr:uid="{7BC68CF8-5A01-47DC-852E-3A474B71A4BD}"/>
+    <hyperlink ref="L146" r:id="rId145" xr:uid="{D980D1A9-4124-46CB-8A21-1075F5C89262}"/>
+    <hyperlink ref="L151" r:id="rId146" xr:uid="{2EE1C1D9-60C6-4933-90B8-FF8D6DB54BE0}"/>
+    <hyperlink ref="L152" r:id="rId147" xr:uid="{7E1F82D2-1487-42CA-8F49-8840CA00D9BD}"/>
+    <hyperlink ref="L153" r:id="rId148" xr:uid="{E9675B85-CCCC-41EC-A374-8B0EEB687ABF}"/>
+    <hyperlink ref="L154" r:id="rId149" xr:uid="{E8CD8B29-C864-43B7-BF17-29C62184BEA9}"/>
+    <hyperlink ref="L155" r:id="rId150" xr:uid="{B95D0080-64D2-4BCA-93D4-1F546B829CEF}"/>
+    <hyperlink ref="L156" r:id="rId151" xr:uid="{F36468A9-7021-46EC-AE95-EB51D2206B9A}"/>
+    <hyperlink ref="L157" r:id="rId152" xr:uid="{7AC1AF03-79E4-4622-B8E2-C18330DC3F9A}"/>
+    <hyperlink ref="L158" r:id="rId153" xr:uid="{609C026B-4ACB-4FF6-AC60-7FD4914093B9}"/>
+    <hyperlink ref="L159" r:id="rId154" xr:uid="{0F4685AB-B355-4755-BF99-0D9A14723E3C}"/>
+    <hyperlink ref="L160" r:id="rId155" xr:uid="{92DBA903-68A3-4B3F-B387-C603065FD408}"/>
+    <hyperlink ref="L161" r:id="rId156" xr:uid="{98210422-88A9-4BBC-A502-66D790D14B92}"/>
+    <hyperlink ref="L162" r:id="rId157" xr:uid="{54696E6F-468E-4145-9AC3-2346E9B34D9B}"/>
+    <hyperlink ref="L163" r:id="rId158" xr:uid="{54556323-7EFA-4D01-81E1-E0A37279D3F7}"/>
+    <hyperlink ref="L164" r:id="rId159" xr:uid="{5BFE94AB-E6AA-4365-BD55-6FBB9850CFDA}"/>
+    <hyperlink ref="L165" r:id="rId160" xr:uid="{19004F54-7141-4C2E-9690-41618876FA29}"/>
+    <hyperlink ref="L166" r:id="rId161" xr:uid="{31BF8CD1-77DC-4417-A338-C593039BFD40}"/>
+    <hyperlink ref="L167" r:id="rId162" xr:uid="{281861A6-0E5B-4881-AA22-D154A05A4E68}"/>
+    <hyperlink ref="L168" r:id="rId163" xr:uid="{4CB61E3D-8D7C-4CA4-A55F-641C3BC3AE7C}"/>
+    <hyperlink ref="L169" r:id="rId164" xr:uid="{00CFECC1-5DFA-4609-A1CD-B71ED5EA1CBF}"/>
+    <hyperlink ref="L170" r:id="rId165" xr:uid="{BFEB6BC8-ECDC-4C0A-B8D1-BF1A847D8069}"/>
+    <hyperlink ref="L171" r:id="rId166" xr:uid="{539A4AEF-AC57-43A0-9020-C812FF490F7D}"/>
+    <hyperlink ref="L172" r:id="rId167" xr:uid="{EE7654BB-8779-4675-8E24-3CA6DFB97FD1}"/>
+    <hyperlink ref="L173" r:id="rId168" xr:uid="{3A0A7DD4-AB2E-43D3-B4F7-69532B719301}"/>
+    <hyperlink ref="L174" r:id="rId169" xr:uid="{0B00404E-0A5F-44A6-BA11-A14521DFA0BB}"/>
+    <hyperlink ref="L175" r:id="rId170" xr:uid="{34BD48A1-CB66-49F8-94E4-886C55257C47}"/>
+    <hyperlink ref="L176" r:id="rId171" xr:uid="{21516EE5-F78A-4CBA-9D6F-635952297241}"/>
+    <hyperlink ref="L177" r:id="rId172" xr:uid="{6E0815BE-46FE-48A8-A9C7-4814D813173A}"/>
+    <hyperlink ref="L178" r:id="rId173" xr:uid="{65F14255-10F7-47A5-A769-0EE75C8B2558}"/>
+    <hyperlink ref="L179" r:id="rId174" xr:uid="{A47E2FAC-4C8C-4097-BD2A-5B1C05BA38B6}"/>
+    <hyperlink ref="L180" r:id="rId175" xr:uid="{0BF73651-8407-4BD9-8ED4-262BB68D10D3}"/>
+    <hyperlink ref="L181" r:id="rId176" xr:uid="{B58C3235-C3DF-4479-A53C-805B95F35C30}"/>
+    <hyperlink ref="L182" r:id="rId177" xr:uid="{F965C7E3-2B53-4324-972E-8980AE14E4D7}"/>
+    <hyperlink ref="L183" r:id="rId178" xr:uid="{58257C62-A81D-446F-B18B-BEF9952F0375}"/>
+    <hyperlink ref="L184" r:id="rId179" xr:uid="{C785A14B-E96C-481B-A138-8C5C0E1F820E}"/>
+    <hyperlink ref="L185" r:id="rId180" xr:uid="{B72CF05A-AA5F-4D93-8125-E83FBD0B8291}"/>
+    <hyperlink ref="L186" r:id="rId181" xr:uid="{AE08C09D-6270-4E2E-9309-581447E4C254}"/>
+    <hyperlink ref="L23" r:id="rId182" xr:uid="{869BD461-8399-4E46-AB5F-BF7FEC22AA98}"/>
+    <hyperlink ref="L122" r:id="rId183" xr:uid="{16C37BC8-D542-42B7-9EE6-2CF4FC678B9F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{71771692-E9E6-45F5-A721-173C71C0A55B}">
           <x14:formula1>
             <xm:f>label!$A:$A</xm:f>
@@ -6736,6 +7455,12 @@
           </x14:formula1>
           <xm:sqref>C2:C1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{142E1B15-4840-422A-BD0C-26D5C3B0A896}">
+          <x14:formula1>
+            <xm:f>source!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>L2:L1048576</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -6744,10 +7469,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B5E982-8B9C-4FA7-94A5-9ED6F96734F4}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6759,36 +7484,31 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
         <v>165</v>
       </c>
     </row>
@@ -6799,10 +7519,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{135DECB3-8050-4A31-957F-61CD3DC80792}">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7207,94 +7927,102 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>29</v>
+        <v>379</v>
       </c>
       <c r="B50" t="s">
-        <v>62</v>
+        <v>380</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>129</v>
+        <v>29</v>
       </c>
       <c r="B51" t="s">
-        <v>130</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>38</v>
+        <v>129</v>
       </c>
       <c r="B52" t="s">
-        <v>64</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>145</v>
+        <v>38</v>
       </c>
       <c r="B53" t="s">
-        <v>146</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>28</v>
+        <v>145</v>
       </c>
       <c r="B54" t="s">
-        <v>65</v>
+        <v>146</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B55" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>82</v>
+        <v>35</v>
       </c>
       <c r="B56" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="B57" t="s">
-        <v>119</v>
+        <v>83</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="B58" t="s">
-        <v>92</v>
+        <v>119</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>147</v>
+        <v>91</v>
       </c>
       <c r="B59" t="s">
-        <v>148</v>
+        <v>92</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>147</v>
+      </c>
+      <c r="B60" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>106</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>107</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:A55">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:A56">
     <sortCondition ref="A22"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7306,11 +8034,17 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>